<commit_message>
Added ISBN to excel sheet
</commit_message>
<xml_diff>
--- a/fullLibrary.xlsx
+++ b/fullLibrary.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Title</t>
   </si>
@@ -31,7 +31,7 @@
     <t>Page Count</t>
   </si>
   <si>
-    <t/>
+    <t>ISBN</t>
   </si>
 </sst>
 </file>
@@ -49,7 +49,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -62,7 +62,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -85,30 +85,20 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -418,20 +408,21 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="4" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="5" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -447,51 +438,9 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>